<commit_message>
cambio en diagrama de CU  y fichas
</commit_message>
<xml_diff>
--- a/Fichas Casos de Uso.xlsx
+++ b/Fichas Casos de Uso.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC76FF-50C2-4709-A105-B6B61D095E5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A57F7E2-2FD7-4AFB-A370-6F12C92B9CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
@@ -175,9 +175,6 @@
     <t>Selecciona el nuevo turno y hora y hace clic en aplicar cambios</t>
   </si>
   <si>
-    <t> Gestionar Tecnicos</t>
-  </si>
-  <si>
     <t>El tecnico debe haber pasado los requisitos solicitados por la empresa</t>
   </si>
   <si>
@@ -226,10 +223,13 @@
     <t>Dar clic en acertar</t>
   </si>
   <si>
-    <t> 002</t>
-  </si>
-  <si>
     <t>Se actualiza la relación del tecnico con el turno y se envia una notificación por correo al tecnico sobre los cambios realizados</t>
+  </si>
+  <si>
+    <t> Registrar Tecnico</t>
+  </si>
+  <si>
+    <t> Cambiar turno</t>
   </si>
 </sst>
 </file>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
   <dimension ref="B2:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89:D89"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="14"/>
     </row>
@@ -1128,7 +1128,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" s="12"/>
     </row>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D65" s="14"/>
     </row>
@@ -1290,7 +1290,7 @@
         <v>6</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D68" s="12"/>
     </row>
@@ -1299,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D69" s="12"/>
     </row>
@@ -1320,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
@@ -1329,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
@@ -1347,7 +1347,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>24</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D83" s="12"/>
     </row>
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D86" s="14"/>
     </row>
@@ -1425,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="D87" s="14"/>
     </row>
@@ -1443,7 +1443,7 @@
         <v>6</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D89" s="12"/>
     </row>
@@ -1452,7 +1452,7 @@
         <v>8</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D90" s="12"/>
     </row>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>2</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -1491,7 +1491,7 @@
         <v>3</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>4</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
         <v>5</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
@@ -1560,12 +1560,44 @@
         <v>24</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D104" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B91:B97"/>
+    <mergeCell ref="B98:B103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="B70:B76"/>
+    <mergeCell ref="B77:B82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B49:B55"/>
     <mergeCell ref="B56:B61"/>
     <mergeCell ref="C62:D62"/>
@@ -1574,38 +1606,6 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B70:B76"/>
-    <mergeCell ref="B77:B82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="B91:B97"/>
-    <mergeCell ref="B98:B103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>